<commit_message>
logea y vuelv   e a agendar con los parámetros correctos
</commit_message>
<xml_diff>
--- a/data/reservas.xlsx
+++ b/data/reservas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto_paw_care\Frontend_paw_care\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto_paw_care\Frontend_paw_care2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3761C25-171D-4CF4-B341-6BC76586EA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48326952-384E-4EA0-8A1F-60F83DDC6554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{152CC9B7-6DBF-4793-B978-7580A77B8391}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,13 +496,13 @@
       </c>
       <c r="F2" s="1">
         <f ca="1">TODAY()</f>
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="G2" s="2">
         <v>0.41666666666666669</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -523,13 +523,13 @@
       </c>
       <c r="F3" s="1">
         <f ca="1">TODAY()</f>
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="G3" s="2">
         <v>0.45833333333333331</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -550,13 +550,13 @@
       </c>
       <c r="F4" s="1">
         <f ca="1">F3+1</f>
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="G4" s="2">
         <v>0.5</v>
       </c>
       <c r="H4">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -577,13 +577,13 @@
       </c>
       <c r="F5" s="1">
         <f ca="1">TODAY()</f>
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="G5" s="2">
         <v>0.54166666666666696</v>
       </c>
       <c r="H5">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
       </c>
       <c r="F6" s="1">
         <f ca="1">TODAY()</f>
-        <v>45742</v>
+        <v>45745</v>
       </c>
       <c r="G6" s="2">
         <v>0.58333333333333404</v>
@@ -631,7 +631,7 @@
       </c>
       <c r="F7" s="1">
         <f ca="1">F6+1</f>
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="G7" s="2">
         <v>0.625</v>
@@ -658,7 +658,7 @@
       </c>
       <c r="F8" s="1">
         <f ca="1">F7+1</f>
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="G8" s="2">
         <v>0.66666666666666696</v>
@@ -685,7 +685,7 @@
       </c>
       <c r="F9" s="1">
         <f ca="1">F8+1</f>
-        <v>45745</v>
+        <v>45748</v>
       </c>
       <c r="G9" s="2">
         <v>0.70833333333333304</v>

</xml_diff>

<commit_message>
Permite seleccioar el tipo de consulta y agendar correctamente
</commit_message>
<xml_diff>
--- a/data/reservas.xlsx
+++ b/data/reservas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto_paw_care\Frontend_paw_care2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48326952-384E-4EA0-8A1F-60F83DDC6554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472B7105-BB83-4891-B872-E3DD09A6D640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{152CC9B7-6DBF-4793-B978-7580A77B8391}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +496,7 @@
       </c>
       <c r="F2" s="1">
         <f ca="1">TODAY()</f>
-        <v>45745</v>
+        <v>45750</v>
       </c>
       <c r="G2" s="2">
         <v>0.41666666666666669</v>
@@ -523,7 +523,7 @@
       </c>
       <c r="F3" s="1">
         <f ca="1">TODAY()</f>
-        <v>45745</v>
+        <v>45750</v>
       </c>
       <c r="G3" s="2">
         <v>0.45833333333333331</v>
@@ -550,7 +550,7 @@
       </c>
       <c r="F4" s="1">
         <f ca="1">F3+1</f>
-        <v>45746</v>
+        <v>45751</v>
       </c>
       <c r="G4" s="2">
         <v>0.5</v>
@@ -577,7 +577,7 @@
       </c>
       <c r="F5" s="1">
         <f ca="1">TODAY()</f>
-        <v>45745</v>
+        <v>45750</v>
       </c>
       <c r="G5" s="2">
         <v>0.54166666666666696</v>
@@ -604,7 +604,7 @@
       </c>
       <c r="F6" s="1">
         <f ca="1">TODAY()</f>
-        <v>45745</v>
+        <v>45750</v>
       </c>
       <c r="G6" s="2">
         <v>0.58333333333333404</v>
@@ -631,7 +631,7 @@
       </c>
       <c r="F7" s="1">
         <f ca="1">F6+1</f>
-        <v>45746</v>
+        <v>45751</v>
       </c>
       <c r="G7" s="2">
         <v>0.625</v>
@@ -658,7 +658,7 @@
       </c>
       <c r="F8" s="1">
         <f ca="1">F7+1</f>
-        <v>45747</v>
+        <v>45752</v>
       </c>
       <c r="G8" s="2">
         <v>0.66666666666666696</v>
@@ -685,7 +685,7 @@
       </c>
       <c r="F9" s="1">
         <f ca="1">F8+1</f>
-        <v>45748</v>
+        <v>45753</v>
       </c>
       <c r="G9" s="2">
         <v>0.70833333333333304</v>

</xml_diff>